<commit_message>
adding data from Sheet 2
</commit_message>
<xml_diff>
--- a/public/rancho_chargers.xlsx
+++ b/public/rancho_chargers.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandonaparicio/Documents/KIGT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karendiaz/Documents/Current Work/kigt-2023/charge-cloud-2023/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A83A84-3D46-7E4E-9280-032813C50DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F582B8-3568-2A48-8F73-BD5476E172B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19780" xr2:uid="{03A3BEA9-CB6A-EF41-9E96-CBA0740E7C02}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{03A3BEA9-CB6A-EF41-9E96-CBA0740E7C02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="128">
   <si>
     <t>__id__</t>
   </si>
@@ -418,12 +417,6 @@
   </si>
   <si>
     <t>duration (seconds)</t>
-  </si>
-  <si>
-    <t>kwH</t>
-  </si>
-  <si>
-    <t>hr</t>
   </si>
   <si>
     <t>kwh</t>
@@ -473,15 +466,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -840,13 +833,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F754FD42-EA44-AB47-A329-E9B14C19B4CE}">
   <dimension ref="A1:AG45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+    <sheetView topLeftCell="S1" workbookViewId="0">
       <selection activeCell="AG2" sqref="AG2:AG45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="28.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="24" max="24" width="16.6640625" customWidth="1"/>
     <col min="25" max="25" width="21" customWidth="1"/>
@@ -859,7 +852,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -956,11 +949,11 @@
         <v>126</v>
       </c>
       <c r="AG1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2" s="3">
         <v>1696653009722</v>
       </c>
       <c r="B2" t="s">
@@ -1050,21 +1043,21 @@
       <c r="AD2">
         <v>204</v>
       </c>
-      <c r="AE2" s="4">
+      <c r="AE2" s="6">
         <f>(AF2/60)/60</f>
         <v>47.963333333333338</v>
       </c>
-      <c r="AF2" s="4">
+      <c r="AF2" s="6">
         <f>AB3-AB2</f>
         <v>172668</v>
       </c>
-      <c r="AG2" s="3">
+      <c r="AG2" s="5">
         <f>(((AA2/1000)*AD2)/1000)*AE2</f>
         <v>269.07430000000005</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="A3" s="3">
         <v>1696824785115</v>
       </c>
       <c r="B3" t="s">
@@ -1154,12 +1147,12 @@
       <c r="AD3">
         <v>0</v>
       </c>
-      <c r="AE3" s="4"/>
-      <c r="AF3" s="4"/>
-      <c r="AG3" s="3"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="5"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="3">
         <v>1696987681716</v>
       </c>
       <c r="B4" t="s">
@@ -1249,21 +1242,21 @@
       <c r="AD4">
         <v>204</v>
       </c>
-      <c r="AE4" s="4">
+      <c r="AE4" s="6">
         <f>(AF4/60)/60</f>
         <v>0.86277777777777775</v>
       </c>
-      <c r="AF4" s="3">
+      <c r="AF4" s="5">
         <f>AB5-AB4</f>
         <v>3106</v>
       </c>
-      <c r="AG4" s="3">
-        <f t="shared" ref="AG4:AG45" si="0">(((AA4/1000)*AD4)/1000)*AE4</f>
+      <c r="AG4" s="5">
+        <f t="shared" ref="AG4" si="0">(((AA4/1000)*AD4)/1000)*AE4</f>
         <v>4.8401833333333331</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
+      <c r="A5" s="3">
         <v>1696990385714</v>
       </c>
       <c r="B5" t="s">
@@ -1353,12 +1346,12 @@
       <c r="AD5">
         <v>0</v>
       </c>
-      <c r="AE5" s="4"/>
-      <c r="AF5" s="3"/>
-      <c r="AG5" s="3"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="3">
         <v>1696996687915</v>
       </c>
       <c r="B6" t="s">
@@ -1448,21 +1441,21 @@
       <c r="AD6">
         <v>204</v>
       </c>
-      <c r="AE6" s="4">
+      <c r="AE6" s="6">
         <f t="shared" ref="AE6" si="1">(AF6/60)/60</f>
         <v>11.510555555555555</v>
       </c>
-      <c r="AF6" s="3">
+      <c r="AF6" s="5">
         <f>AB7-AB6</f>
         <v>41438</v>
       </c>
-      <c r="AG6" s="3">
-        <f t="shared" ref="AG6:AG45" si="2">(((AA6/1000)*AD6)/1000)*AE6</f>
+      <c r="AG6" s="5">
+        <f t="shared" ref="AG6" si="2">(((AA6/1000)*AD6)/1000)*AE6</f>
         <v>64.574216666666672</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+      <c r="A7" s="3">
         <v>1697038082242</v>
       </c>
       <c r="B7" t="s">
@@ -1552,12 +1545,12 @@
       <c r="AD7">
         <v>0</v>
       </c>
-      <c r="AE7" s="4"/>
-      <c r="AF7" s="3"/>
-      <c r="AG7" s="3"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="5"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8" s="3">
         <v>1697309889216</v>
       </c>
       <c r="B8" t="s">
@@ -1647,21 +1640,21 @@
       <c r="AD8">
         <v>204</v>
       </c>
-      <c r="AE8" s="4">
+      <c r="AE8" s="6">
         <f t="shared" ref="AE8" si="3">(AF8/60)/60</f>
         <v>0.61444444444444446</v>
       </c>
-      <c r="AF8" s="4">
+      <c r="AF8" s="6">
         <f>AB9-AB8</f>
         <v>2212</v>
       </c>
-      <c r="AG8" s="3">
-        <f t="shared" ref="AG8:AG45" si="4">(((AA8/1000)*AD8)/1000)*AE8</f>
+      <c r="AG8" s="5">
+        <f t="shared" ref="AG8" si="4">(((AA8/1000)*AD8)/1000)*AE8</f>
         <v>3.4470333333333336</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+      <c r="A9" s="3">
         <v>1697312588515</v>
       </c>
       <c r="B9" t="s">
@@ -1751,12 +1744,12 @@
       <c r="AD9">
         <v>0</v>
       </c>
-      <c r="AE9" s="4"/>
-      <c r="AF9" s="4"/>
-      <c r="AG9" s="3"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6"/>
+      <c r="AG9" s="5"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
+      <c r="A10" s="3">
         <v>1697421490315</v>
       </c>
       <c r="B10" t="s">
@@ -1846,21 +1839,21 @@
       <c r="AD10" s="1">
         <v>204</v>
       </c>
-      <c r="AE10" s="4">
+      <c r="AE10" s="6">
         <f t="shared" ref="AE10" si="5">(AF10/60)/60</f>
         <v>13.886944444444445</v>
       </c>
-      <c r="AF10" s="3">
+      <c r="AF10" s="5">
         <f>AB11-AB10</f>
         <v>49993</v>
       </c>
-      <c r="AG10" s="3">
-        <f t="shared" ref="AG10:AG45" si="6">(((AA10/1000)*AD10)/1000)*AE10</f>
+      <c r="AG10" s="5">
+        <f t="shared" ref="AG10" si="6">(((AA10/1000)*AD10)/1000)*AE10</f>
         <v>77.905758333333338</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+      <c r="A11" s="3">
         <v>1697471882326</v>
       </c>
       <c r="B11" t="s">
@@ -1950,12 +1943,12 @@
       <c r="AD11">
         <v>0</v>
       </c>
-      <c r="AE11" s="4"/>
-      <c r="AF11" s="3"/>
-      <c r="AG11" s="3"/>
+      <c r="AE11" s="6"/>
+      <c r="AF11" s="5"/>
+      <c r="AG11" s="5"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
+      <c r="A12" s="3">
         <v>1697664492915</v>
       </c>
       <c r="B12" t="s">
@@ -2045,21 +2038,21 @@
       <c r="AD12" s="1">
         <v>204</v>
       </c>
-      <c r="AE12" s="4">
+      <c r="AE12" s="6">
         <f t="shared" ref="AE12" si="7">(AF12/60)/60</f>
         <v>16.593055555555555</v>
       </c>
-      <c r="AF12" s="3">
+      <c r="AF12" s="5">
         <f>AB13-AB12</f>
         <v>59735</v>
       </c>
-      <c r="AG12" s="3">
-        <f t="shared" ref="AG12:AG45" si="8">(((AA12/1000)*AD12)/1000)*AE12</f>
+      <c r="AG12" s="5">
+        <f t="shared" ref="AG12" si="8">(((AA12/1000)*AD12)/1000)*AE12</f>
         <v>93.087041666666664</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
+      <c r="A13" s="3">
         <v>1697724791618</v>
       </c>
       <c r="B13" t="s">
@@ -2149,12 +2142,12 @@
       <c r="AD13" s="1">
         <v>0</v>
       </c>
-      <c r="AE13" s="4"/>
-      <c r="AF13" s="3"/>
-      <c r="AG13" s="3"/>
+      <c r="AE13" s="6"/>
+      <c r="AF13" s="5"/>
+      <c r="AG13" s="5"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
+      <c r="A14" s="3">
         <v>1697967793635</v>
       </c>
       <c r="B14" t="s">
@@ -2244,21 +2237,21 @@
       <c r="AD14" s="1">
         <v>204</v>
       </c>
-      <c r="AE14" s="4">
+      <c r="AE14" s="6">
         <f t="shared" ref="AE14" si="9">(AF14/60)/60</f>
         <v>7.7072222222222226</v>
       </c>
-      <c r="AF14" s="4">
+      <c r="AF14" s="6">
         <f>AB15-AB14</f>
         <v>27746</v>
       </c>
-      <c r="AG14" s="3">
-        <f t="shared" ref="AG14:AG45" si="10">(((AA14/1000)*AD14)/1000)*AE14</f>
+      <c r="AG14" s="5">
+        <f t="shared" ref="AG14" si="10">(((AA14/1000)*AD14)/1000)*AE14</f>
         <v>43.237516666666671</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
+      <c r="A15" s="3">
         <v>1697986686835</v>
       </c>
       <c r="B15" t="s">
@@ -2348,12 +2341,12 @@
       <c r="AD15">
         <v>0</v>
       </c>
-      <c r="AE15" s="4"/>
-      <c r="AF15" s="4"/>
-      <c r="AG15" s="3"/>
+      <c r="AE15" s="6"/>
+      <c r="AF15" s="6"/>
+      <c r="AG15" s="5"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
+      <c r="A16" s="3">
         <v>1698013683434</v>
       </c>
       <c r="B16" t="s">
@@ -2443,21 +2436,21 @@
       <c r="AD16" s="1">
         <v>204</v>
       </c>
-      <c r="AE16" s="4">
+      <c r="AE16" s="6">
         <f t="shared" ref="AE16" si="11">(AF16/60)/60</f>
         <v>21.195833333333333</v>
       </c>
-      <c r="AF16" s="3">
+      <c r="AF16" s="5">
         <f>AB17-AB16</f>
         <v>76305</v>
       </c>
-      <c r="AG16" s="3">
-        <f t="shared" ref="AG16:AG45" si="12">(((AA16/1000)*AD16)/1000)*AE16</f>
+      <c r="AG16" s="5">
+        <f t="shared" ref="AG16" si="12">(((AA16/1000)*AD16)/1000)*AE16</f>
         <v>118.908625</v>
       </c>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
+      <c r="A17" s="3">
         <v>1698090204807</v>
       </c>
       <c r="B17" t="s">
@@ -2547,12 +2540,12 @@
       <c r="AD17">
         <v>0</v>
       </c>
-      <c r="AE17" s="4"/>
-      <c r="AF17" s="3"/>
-      <c r="AG17" s="3"/>
+      <c r="AE17" s="6"/>
+      <c r="AF17" s="5"/>
+      <c r="AG17" s="5"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
+      <c r="A18" s="3">
         <v>1699920788820</v>
       </c>
       <c r="B18" t="s">
@@ -2642,21 +2635,21 @@
       <c r="AD18">
         <v>204</v>
       </c>
-      <c r="AE18" s="4">
+      <c r="AE18" s="6">
         <f t="shared" ref="AE18" si="13">(AF18/60)/60</f>
         <v>12.776944444444444</v>
       </c>
-      <c r="AF18" s="4">
+      <c r="AF18" s="6">
         <f>AB19-AB18</f>
         <v>45997</v>
       </c>
-      <c r="AG18" s="3">
-        <f t="shared" ref="AG18:AG45" si="14">(((AA18/1000)*AD18)/1000)*AE18</f>
+      <c r="AG18" s="5">
+        <f t="shared" ref="AG18" si="14">(((AA18/1000)*AD18)/1000)*AE18</f>
         <v>71.678658333333331</v>
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
+      <c r="A19" s="3">
         <v>1699966682131</v>
       </c>
       <c r="B19" t="s">
@@ -2746,12 +2739,12 @@
       <c r="AD19">
         <v>0</v>
       </c>
-      <c r="AE19" s="4"/>
-      <c r="AF19" s="4"/>
-      <c r="AG19" s="3"/>
+      <c r="AE19" s="6"/>
+      <c r="AF19" s="6"/>
+      <c r="AG19" s="5"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A20" s="5">
+      <c r="A20" s="3">
         <v>1700377084133</v>
       </c>
       <c r="B20" t="s">
@@ -2841,21 +2834,21 @@
       <c r="AD20">
         <v>204</v>
       </c>
-      <c r="AE20" s="4">
+      <c r="AE20" s="6">
         <f t="shared" ref="AE20" si="15">(AF20/60)/60</f>
         <v>15.621388888888889</v>
       </c>
-      <c r="AF20" s="3">
+      <c r="AF20" s="5">
         <f>AB21-AB20</f>
         <v>56237</v>
       </c>
-      <c r="AG20" s="3">
-        <f t="shared" ref="AG20:AG45" si="16">(((AA20/1000)*AD20)/1000)*AE20</f>
+      <c r="AG20" s="5">
+        <f t="shared" ref="AG20" si="16">(((AA20/1000)*AD20)/1000)*AE20</f>
         <v>87.635991666666669</v>
       </c>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
+      <c r="A21" s="3">
         <v>1700433788331</v>
       </c>
       <c r="B21" t="s">
@@ -2945,12 +2938,12 @@
       <c r="AD21">
         <v>0</v>
       </c>
-      <c r="AE21" s="4"/>
-      <c r="AF21" s="3"/>
-      <c r="AG21" s="3"/>
+      <c r="AE21" s="6"/>
+      <c r="AF21" s="5"/>
+      <c r="AG21" s="5"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A22" s="5">
+      <c r="A22" s="3">
         <v>1700726284729</v>
       </c>
       <c r="B22" t="s">
@@ -3040,21 +3033,21 @@
       <c r="AD22">
         <v>204</v>
       </c>
-      <c r="AE22" s="4">
+      <c r="AE22" s="6">
         <f t="shared" ref="AE22" si="17">(AF22/60)/60</f>
         <v>12.109166666666665</v>
       </c>
-      <c r="AF22" s="3">
+      <c r="AF22" s="5">
         <f>AB23-AB22</f>
         <v>43593</v>
       </c>
-      <c r="AG22" s="3">
-        <f t="shared" ref="AG22:AG45" si="18">(((AA22/1000)*AD22)/1000)*AE22</f>
+      <c r="AG22" s="5">
+        <f t="shared" ref="AG22" si="18">(((AA22/1000)*AD22)/1000)*AE22</f>
         <v>67.932424999999995</v>
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A23" s="5">
+      <c r="A23" s="3">
         <v>1700769483830</v>
       </c>
       <c r="B23" t="s">
@@ -3144,12 +3137,12 @@
       <c r="AD23">
         <v>0</v>
       </c>
-      <c r="AE23" s="4"/>
-      <c r="AF23" s="3"/>
-      <c r="AG23" s="3"/>
+      <c r="AE23" s="6"/>
+      <c r="AF23" s="5"/>
+      <c r="AG23" s="5"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A24" s="5">
+      <c r="A24" s="3">
         <v>1701065585929</v>
       </c>
       <c r="B24" t="s">
@@ -3239,21 +3232,21 @@
       <c r="AD24">
         <v>204</v>
       </c>
-      <c r="AE24" s="4">
+      <c r="AE24" s="6">
         <f t="shared" ref="AE24" si="19">(AF24/60)/60</f>
         <v>9.6841666666666661</v>
       </c>
-      <c r="AF24" s="3">
+      <c r="AF24" s="5">
         <f>AB25-AB24</f>
         <v>34863</v>
       </c>
-      <c r="AG24" s="3">
-        <f t="shared" ref="AG24:AG45" si="20">(((AA24/1000)*AD24)/1000)*AE24</f>
+      <c r="AG24" s="5">
+        <f t="shared" ref="AG24" si="20">(((AA24/1000)*AD24)/1000)*AE24</f>
         <v>54.328175000000002</v>
       </c>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A25" s="5">
+      <c r="A25" s="3">
         <v>1701101592629</v>
       </c>
       <c r="B25" t="s">
@@ -3343,12 +3336,12 @@
       <c r="AD25">
         <v>0</v>
       </c>
-      <c r="AE25" s="4"/>
-      <c r="AF25" s="3"/>
-      <c r="AG25" s="3"/>
+      <c r="AE25" s="6"/>
+      <c r="AF25" s="5"/>
+      <c r="AG25" s="5"/>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A26" s="5">
+      <c r="A26" s="3">
         <v>1701333782302</v>
       </c>
       <c r="B26" t="s">
@@ -3438,21 +3431,21 @@
       <c r="AD26">
         <v>204</v>
       </c>
-      <c r="AE26" s="4">
+      <c r="AE26" s="6">
         <f t="shared" ref="AE26" si="21">(AF26/60)/60</f>
         <v>9.1169444444444441</v>
       </c>
-      <c r="AF26" s="4">
+      <c r="AF26" s="6">
         <f>AB27-AB26</f>
         <v>32821</v>
       </c>
-      <c r="AG26" s="3">
-        <f t="shared" ref="AG26:AG45" si="22">(((AA26/1000)*AD26)/1000)*AE26</f>
+      <c r="AG26" s="5">
+        <f t="shared" ref="AG26" si="22">(((AA26/1000)*AD26)/1000)*AE26</f>
         <v>51.146058333333336</v>
       </c>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A27" s="5">
+      <c r="A27" s="3">
         <v>1701367087504</v>
       </c>
       <c r="B27" t="s">
@@ -3542,12 +3535,12 @@
       <c r="AD27">
         <v>0</v>
       </c>
-      <c r="AE27" s="4"/>
-      <c r="AF27" s="4"/>
-      <c r="AG27" s="3"/>
+      <c r="AE27" s="6"/>
+      <c r="AF27" s="6"/>
+      <c r="AG27" s="5"/>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A28" s="5">
+      <c r="A28" s="3">
         <v>1701585786916</v>
       </c>
       <c r="B28" t="s">
@@ -3637,21 +3630,21 @@
       <c r="AD28">
         <v>204</v>
       </c>
-      <c r="AE28" s="4">
+      <c r="AE28" s="6">
         <f t="shared" ref="AE28" si="23">(AF28/60)/60</f>
         <v>11.195833333333333</v>
       </c>
-      <c r="AF28" s="3">
+      <c r="AF28" s="5">
         <f>AB29-AB28</f>
         <v>40305</v>
       </c>
-      <c r="AG28" s="3">
-        <f t="shared" ref="AG28:AG45" si="24">(((AA28/1000)*AD28)/1000)*AE28</f>
+      <c r="AG28" s="5">
+        <f t="shared" ref="AG28" si="24">(((AA28/1000)*AD28)/1000)*AE28</f>
         <v>62.808624999999999</v>
       </c>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A29" s="5">
+      <c r="A29" s="3">
         <v>1701626282132</v>
       </c>
       <c r="B29" t="s">
@@ -3741,12 +3734,12 @@
       <c r="AD29">
         <v>0</v>
       </c>
-      <c r="AE29" s="4"/>
-      <c r="AF29" s="3"/>
-      <c r="AG29" s="3"/>
+      <c r="AE29" s="6"/>
+      <c r="AF29" s="5"/>
+      <c r="AG29" s="5"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A30" s="5">
+      <c r="A30" s="3">
         <v>1701658682217</v>
       </c>
       <c r="B30" t="s">
@@ -3836,21 +3829,21 @@
       <c r="AD30">
         <v>204</v>
       </c>
-      <c r="AE30" s="4">
+      <c r="AE30" s="6">
         <f t="shared" ref="AE30" si="25">(AF30/60)/60</f>
         <v>0.23138888888888889</v>
       </c>
-      <c r="AF30" s="3">
+      <c r="AF30" s="5">
         <f>AB31-AB30</f>
         <v>833</v>
       </c>
-      <c r="AG30" s="3">
-        <f t="shared" ref="AG30:AG45" si="26">(((AA30/1000)*AD30)/1000)*AE30</f>
+      <c r="AG30" s="5">
+        <f t="shared" ref="AG30" si="26">(((AA30/1000)*AD30)/1000)*AE30</f>
         <v>1.2980916666666669</v>
       </c>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A31" s="5">
+      <c r="A31" s="3">
         <v>1701659581815</v>
       </c>
       <c r="B31" t="s">
@@ -3940,12 +3933,12 @@
       <c r="AD31">
         <v>0</v>
       </c>
-      <c r="AE31" s="4"/>
-      <c r="AF31" s="3"/>
-      <c r="AG31" s="3"/>
+      <c r="AE31" s="6"/>
+      <c r="AF31" s="5"/>
+      <c r="AG31" s="5"/>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A32" s="5">
+      <c r="A32" s="3">
         <v>1701669482116</v>
       </c>
       <c r="B32" t="s">
@@ -4035,21 +4028,21 @@
       <c r="AD32">
         <v>204</v>
       </c>
-      <c r="AE32" s="4">
+      <c r="AE32" s="6">
         <f t="shared" ref="AE32" si="27">(AF32/60)/60</f>
         <v>13.844444444444443</v>
       </c>
-      <c r="AF32" s="4">
+      <c r="AF32" s="6">
         <f>AB33-AB32</f>
         <v>49840</v>
       </c>
-      <c r="AG32" s="3">
-        <f t="shared" ref="AG32:AG45" si="28">(((AA32/1000)*AD32)/1000)*AE32</f>
+      <c r="AG32" s="5">
+        <f t="shared" ref="AG32" si="28">(((AA32/1000)*AD32)/1000)*AE32</f>
         <v>77.667333333333332</v>
       </c>
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A33" s="5">
+      <c r="A33" s="3">
         <v>1701718995015</v>
       </c>
       <c r="B33" t="s">
@@ -4139,12 +4132,12 @@
       <c r="AD33">
         <v>0</v>
       </c>
-      <c r="AE33" s="4"/>
-      <c r="AF33" s="4"/>
-      <c r="AG33" s="3"/>
+      <c r="AE33" s="6"/>
+      <c r="AF33" s="6"/>
+      <c r="AG33" s="5"/>
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A34" s="5">
+      <c r="A34" s="3">
         <v>1701743281925</v>
       </c>
       <c r="B34" t="s">
@@ -4234,21 +4227,21 @@
       <c r="AD34">
         <v>204</v>
       </c>
-      <c r="AE34" s="4">
+      <c r="AE34" s="6">
         <f t="shared" ref="AE34" si="29">(AF34/60)/60</f>
         <v>14.022500000000001</v>
       </c>
-      <c r="AF34" s="3">
+      <c r="AF34" s="5">
         <f>AB35-AB34</f>
         <v>50481</v>
       </c>
-      <c r="AG34" s="3">
-        <f t="shared" ref="AG34:AG45" si="30">(((AA34/1000)*AD34)/1000)*AE34</f>
+      <c r="AG34" s="5">
+        <f t="shared" ref="AG34" si="30">(((AA34/1000)*AD34)/1000)*AE34</f>
         <v>78.666225000000011</v>
       </c>
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A35" s="5">
+      <c r="A35" s="3">
         <v>1701856815102</v>
       </c>
       <c r="B35" t="s">
@@ -4338,12 +4331,12 @@
       <c r="AD35">
         <v>0</v>
       </c>
-      <c r="AE35" s="4"/>
-      <c r="AF35" s="3"/>
-      <c r="AG35" s="3"/>
+      <c r="AE35" s="6"/>
+      <c r="AF35" s="5"/>
+      <c r="AG35" s="5"/>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A36" s="5">
+      <c r="A36" s="3">
         <v>1701935882919</v>
       </c>
       <c r="B36" t="s">
@@ -4433,21 +4426,21 @@
       <c r="AD36">
         <v>204</v>
       </c>
-      <c r="AE36" s="4">
+      <c r="AE36" s="6">
         <f t="shared" ref="AE36" si="31">(AF36/60)/60</f>
         <v>20.946666666666665</v>
       </c>
-      <c r="AF36" s="3">
+      <c r="AF36" s="5">
         <f>AB37-AB36</f>
         <v>75408</v>
       </c>
-      <c r="AG36" s="3">
-        <f t="shared" ref="AG36:AG45" si="32">(((AA36/1000)*AD36)/1000)*AE36</f>
+      <c r="AG36" s="5">
+        <f t="shared" ref="AG36" si="32">(((AA36/1000)*AD36)/1000)*AE36</f>
         <v>117.5108</v>
       </c>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A37" s="5">
+      <c r="A37" s="3">
         <v>1702011484335</v>
       </c>
       <c r="B37" t="s">
@@ -4537,12 +4530,12 @@
       <c r="AD37">
         <v>0</v>
       </c>
-      <c r="AE37" s="4"/>
-      <c r="AF37" s="3"/>
-      <c r="AG37" s="3"/>
+      <c r="AE37" s="6"/>
+      <c r="AF37" s="5"/>
+      <c r="AG37" s="5"/>
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A38" s="5">
+      <c r="A38" s="3">
         <v>1702209614899</v>
       </c>
       <c r="B38" t="s">
@@ -4632,21 +4625,21 @@
       <c r="AD38">
         <v>204</v>
       </c>
-      <c r="AE38" s="4">
+      <c r="AE38" s="6">
         <f t="shared" ref="AE38" si="33">(AF38/60)/60</f>
         <v>11.537777777777778</v>
       </c>
-      <c r="AF38" s="4">
+      <c r="AF38" s="6">
         <f>AB39-AB38</f>
         <v>41536</v>
       </c>
-      <c r="AG38" s="3">
-        <f t="shared" ref="AG38:AG45" si="34">(((AA38/1000)*AD38)/1000)*AE38</f>
+      <c r="AG38" s="5">
+        <f t="shared" ref="AG38" si="34">(((AA38/1000)*AD38)/1000)*AE38</f>
         <v>64.726933333333335</v>
       </c>
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A39" s="5">
+      <c r="A39" s="3">
         <v>1702289727297</v>
       </c>
       <c r="B39" t="s">
@@ -4736,12 +4729,12 @@
       <c r="AD39">
         <v>0</v>
       </c>
-      <c r="AE39" s="4"/>
-      <c r="AF39" s="4"/>
-      <c r="AG39" s="3"/>
+      <c r="AE39" s="6"/>
+      <c r="AF39" s="6"/>
+      <c r="AG39" s="5"/>
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A40" s="5">
+      <c r="A40" s="3">
         <v>1702345382209</v>
       </c>
       <c r="B40" t="s">
@@ -4831,21 +4824,21 @@
       <c r="AD40">
         <v>204</v>
       </c>
-      <c r="AE40" s="4">
+      <c r="AE40" s="6">
         <f t="shared" ref="AE40" si="35">(AF40/60)/60</f>
         <v>16.225277777777777</v>
       </c>
-      <c r="AF40" s="3">
+      <c r="AF40" s="5">
         <f>AB41-AB40</f>
         <v>58411</v>
       </c>
-      <c r="AG40" s="3">
-        <f t="shared" ref="AG40:AG45" si="36">(((AA40/1000)*AD40)/1000)*AE40</f>
+      <c r="AG40" s="5">
+        <f t="shared" ref="AG40" si="36">(((AA40/1000)*AD40)/1000)*AE40</f>
         <v>91.023808333333335</v>
       </c>
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A41" s="5">
+      <c r="A41" s="3">
         <v>1702403881615</v>
       </c>
       <c r="B41" t="s">
@@ -4935,12 +4928,12 @@
       <c r="AD41">
         <v>0</v>
       </c>
-      <c r="AE41" s="4"/>
-      <c r="AF41" s="3"/>
-      <c r="AG41" s="3"/>
+      <c r="AE41" s="6"/>
+      <c r="AF41" s="5"/>
+      <c r="AG41" s="5"/>
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A42" s="5">
+      <c r="A42" s="3">
         <v>1702453386299</v>
       </c>
       <c r="B42" t="s">
@@ -5030,21 +5023,21 @@
       <c r="AD42">
         <v>204</v>
       </c>
-      <c r="AE42" s="4">
+      <c r="AE42" s="6">
         <f>(AF42/60)/60</f>
         <v>8.3838888888888885</v>
       </c>
-      <c r="AF42" s="3">
+      <c r="AF42" s="5">
         <f>AB43-AB42</f>
         <v>30182</v>
       </c>
-      <c r="AG42" s="3">
-        <f t="shared" ref="AG42:AG45" si="37">(((AA42/1000)*AD42)/1000)*AE42</f>
+      <c r="AG42" s="5">
+        <f t="shared" ref="AG42" si="37">(((AA42/1000)*AD42)/1000)*AE42</f>
         <v>47.033616666666667</v>
       </c>
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A43" s="5">
+      <c r="A43" s="3">
         <v>1702483090398</v>
       </c>
       <c r="B43" t="s">
@@ -5134,12 +5127,12 @@
       <c r="AD43">
         <v>0</v>
       </c>
-      <c r="AE43" s="4"/>
-      <c r="AF43" s="3"/>
-      <c r="AG43" s="3"/>
+      <c r="AE43" s="6"/>
+      <c r="AF43" s="5"/>
+      <c r="AG43" s="5"/>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A44" s="5">
+      <c r="A44" s="3">
         <v>1702528983319</v>
       </c>
       <c r="B44" t="s">
@@ -5229,21 +5222,21 @@
       <c r="AD44">
         <v>204</v>
       </c>
-      <c r="AE44" s="4">
+      <c r="AE44" s="6">
         <f>(AF44/60)/60</f>
         <v>12.232777777777779</v>
       </c>
-      <c r="AF44" s="3">
+      <c r="AF44" s="5">
         <f>AB45-AB44</f>
         <v>44038</v>
       </c>
-      <c r="AG44" s="3">
-        <f t="shared" ref="AG44:AG45" si="38">(((AA44/1000)*AD44)/1000)*AE44</f>
+      <c r="AG44" s="5">
+        <f t="shared" ref="AG44" si="38">(((AA44/1000)*AD44)/1000)*AE44</f>
         <v>68.625883333333348</v>
       </c>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A45" s="5">
+      <c r="A45" s="3">
         <v>1702572200899</v>
       </c>
       <c r="B45" t="s">
@@ -5333,50 +5326,24 @@
       <c r="AD45">
         <v>0</v>
       </c>
-      <c r="AE45" s="4"/>
-      <c r="AF45" s="3"/>
-      <c r="AG45" s="3"/>
+      <c r="AE45" s="6"/>
+      <c r="AF45" s="5"/>
+      <c r="AG45" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="66">
-    <mergeCell ref="AG40:AG41"/>
-    <mergeCell ref="AG42:AG43"/>
-    <mergeCell ref="AG44:AG45"/>
-    <mergeCell ref="AG26:AG27"/>
-    <mergeCell ref="AG28:AG29"/>
-    <mergeCell ref="AG30:AG31"/>
-    <mergeCell ref="AG32:AG33"/>
-    <mergeCell ref="AG34:AG35"/>
-    <mergeCell ref="AG36:AG37"/>
-    <mergeCell ref="AG38:AG39"/>
-    <mergeCell ref="AG14:AG15"/>
-    <mergeCell ref="AG16:AG17"/>
-    <mergeCell ref="AG18:AG19"/>
-    <mergeCell ref="AG20:AG21"/>
-    <mergeCell ref="AG22:AG23"/>
-    <mergeCell ref="AG24:AG25"/>
-    <mergeCell ref="AF38:AF39"/>
-    <mergeCell ref="AF40:AF41"/>
-    <mergeCell ref="AF42:AF43"/>
-    <mergeCell ref="AF44:AF45"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AG4:AG5"/>
-    <mergeCell ref="AG6:AG7"/>
-    <mergeCell ref="AG8:AG9"/>
-    <mergeCell ref="AG10:AG11"/>
-    <mergeCell ref="AG12:AG13"/>
-    <mergeCell ref="AF26:AF27"/>
-    <mergeCell ref="AF28:AF29"/>
-    <mergeCell ref="AF30:AF31"/>
-    <mergeCell ref="AF32:AF33"/>
-    <mergeCell ref="AF34:AF35"/>
-    <mergeCell ref="AF36:AF37"/>
-    <mergeCell ref="AF14:AF15"/>
-    <mergeCell ref="AF16:AF17"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AF20:AF21"/>
-    <mergeCell ref="AF22:AF23"/>
-    <mergeCell ref="AF24:AF25"/>
+    <mergeCell ref="AE24:AE25"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AE4:AE5"/>
+    <mergeCell ref="AE6:AE7"/>
+    <mergeCell ref="AE8:AE9"/>
+    <mergeCell ref="AE10:AE11"/>
+    <mergeCell ref="AE12:AE13"/>
+    <mergeCell ref="AE14:AE15"/>
+    <mergeCell ref="AE16:AE17"/>
+    <mergeCell ref="AE18:AE19"/>
+    <mergeCell ref="AE20:AE21"/>
+    <mergeCell ref="AE22:AE23"/>
     <mergeCell ref="AE38:AE39"/>
     <mergeCell ref="AE40:AE41"/>
     <mergeCell ref="AE42:AE43"/>
@@ -5393,18 +5360,44 @@
     <mergeCell ref="AE32:AE33"/>
     <mergeCell ref="AE34:AE35"/>
     <mergeCell ref="AE36:AE37"/>
-    <mergeCell ref="AE14:AE15"/>
-    <mergeCell ref="AE16:AE17"/>
-    <mergeCell ref="AE18:AE19"/>
-    <mergeCell ref="AE20:AE21"/>
-    <mergeCell ref="AE22:AE23"/>
-    <mergeCell ref="AE24:AE25"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AE4:AE5"/>
-    <mergeCell ref="AE6:AE7"/>
-    <mergeCell ref="AE8:AE9"/>
-    <mergeCell ref="AE10:AE11"/>
-    <mergeCell ref="AE12:AE13"/>
+    <mergeCell ref="AG12:AG13"/>
+    <mergeCell ref="AF26:AF27"/>
+    <mergeCell ref="AF28:AF29"/>
+    <mergeCell ref="AF30:AF31"/>
+    <mergeCell ref="AF32:AF33"/>
+    <mergeCell ref="AF14:AF15"/>
+    <mergeCell ref="AF16:AF17"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AF20:AF21"/>
+    <mergeCell ref="AF22:AF23"/>
+    <mergeCell ref="AF24:AF25"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AG4:AG5"/>
+    <mergeCell ref="AG6:AG7"/>
+    <mergeCell ref="AG8:AG9"/>
+    <mergeCell ref="AG10:AG11"/>
+    <mergeCell ref="AG24:AG25"/>
+    <mergeCell ref="AF38:AF39"/>
+    <mergeCell ref="AF40:AF41"/>
+    <mergeCell ref="AF42:AF43"/>
+    <mergeCell ref="AF44:AF45"/>
+    <mergeCell ref="AF34:AF35"/>
+    <mergeCell ref="AF36:AF37"/>
+    <mergeCell ref="AG14:AG15"/>
+    <mergeCell ref="AG16:AG17"/>
+    <mergeCell ref="AG18:AG19"/>
+    <mergeCell ref="AG20:AG21"/>
+    <mergeCell ref="AG22:AG23"/>
+    <mergeCell ref="AG40:AG41"/>
+    <mergeCell ref="AG42:AG43"/>
+    <mergeCell ref="AG44:AG45"/>
+    <mergeCell ref="AG26:AG27"/>
+    <mergeCell ref="AG28:AG29"/>
+    <mergeCell ref="AG30:AG31"/>
+    <mergeCell ref="AG32:AG33"/>
+    <mergeCell ref="AG34:AG35"/>
+    <mergeCell ref="AG36:AG37"/>
+    <mergeCell ref="AG38:AG39"/>
   </mergeCells>
   <conditionalFormatting sqref="K1:K45">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="03^00">
@@ -5422,8 +5415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F40127-0582-344F-8FE6-68861E1DBA5C}">
   <dimension ref="A1:AG23"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AL19" sqref="AL19"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AE10" sqref="AE10:AE11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5451,7 +5444,7 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F1" t="s">
@@ -5533,7 +5526,7 @@
         <v>126</v>
       </c>
       <c r="AF1" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="AG1" t="s">
         <v>127</v>
@@ -5552,7 +5545,7 @@
       <c r="D2">
         <v>20061983802</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="3">
         <v>20231007034825</v>
       </c>
       <c r="F2" t="b">
@@ -5630,15 +5623,15 @@
       <c r="AD2">
         <v>204</v>
       </c>
-      <c r="AE2" s="4">
+      <c r="AE2" s="6">
         <f>AB3-AB2</f>
         <v>36717</v>
       </c>
-      <c r="AF2" s="3">
+      <c r="AF2" s="5">
         <f>(AE2/60)/60</f>
         <v>10.199166666666667</v>
       </c>
-      <c r="AG2" s="3">
+      <c r="AG2" s="5">
         <f>(((AA2/1000)*AD2)/1000)*AF2</f>
         <v>57.217325000000002</v>
       </c>
@@ -5656,7 +5649,7 @@
       <c r="D3">
         <v>20061983802</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>20231007034825</v>
       </c>
       <c r="F3" t="b">
@@ -5734,9 +5727,9 @@
       <c r="AD3">
         <v>0</v>
       </c>
-      <c r="AE3" s="4"/>
-      <c r="AF3" s="3"/>
-      <c r="AG3" s="3"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="5"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -5751,7 +5744,7 @@
       <c r="D4">
         <v>20069701802</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>20231008184212</v>
       </c>
       <c r="F4" t="b">
@@ -5829,15 +5822,15 @@
       <c r="AD4">
         <v>204</v>
       </c>
-      <c r="AE4" s="3">
+      <c r="AE4" s="5">
         <f>AB5-AB4</f>
         <v>51241</v>
       </c>
-      <c r="AF4" s="3">
+      <c r="AF4" s="5">
         <f>(AE4/60)/60</f>
         <v>14.233611111111111</v>
       </c>
-      <c r="AG4" s="3">
+      <c r="AG4" s="5">
         <f>(((AA4/1000)*AD4)/1000)*AF4</f>
         <v>79.850558333333339</v>
       </c>
@@ -5855,7 +5848,7 @@
       <c r="D5">
         <v>20069701802</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>20231008184212</v>
       </c>
       <c r="F5" t="b">
@@ -5933,9 +5926,9 @@
       <c r="AD5">
         <v>0</v>
       </c>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
-      <c r="AG5" s="3"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -5950,7 +5943,7 @@
       <c r="D6">
         <v>20105419103</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>20231013221219</v>
       </c>
       <c r="F6" t="b">
@@ -6028,15 +6021,15 @@
       <c r="AD6">
         <v>204</v>
       </c>
-      <c r="AE6" s="3">
+      <c r="AE6" s="5">
         <f>AB7-AB6</f>
         <v>52268</v>
       </c>
-      <c r="AF6" s="3">
+      <c r="AF6" s="5">
         <f t="shared" ref="AF6" si="0">(AE6/60)/60</f>
         <v>14.518888888888888</v>
       </c>
-      <c r="AG6" s="3">
+      <c r="AG6" s="5">
         <f>(((AA6/1000)*AD6)/1000)*AF6</f>
         <v>81.450966666666673</v>
       </c>
@@ -6054,7 +6047,7 @@
       <c r="D7">
         <v>20105419103</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>20231013221219</v>
       </c>
       <c r="F7" t="b">
@@ -6132,9 +6125,9 @@
       <c r="AD7">
         <v>0</v>
       </c>
-      <c r="AE7" s="3"/>
-      <c r="AF7" s="3"/>
-      <c r="AG7" s="3"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="5"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
@@ -6149,7 +6142,7 @@
       <c r="D8">
         <v>20359524403</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>20231123171042</v>
       </c>
       <c r="F8" t="b">
@@ -6227,15 +6220,15 @@
       <c r="AD8">
         <v>204</v>
       </c>
-      <c r="AE8" s="4">
+      <c r="AE8" s="6">
         <f>AB9-AB8</f>
         <v>1715</v>
       </c>
-      <c r="AF8" s="3">
+      <c r="AF8" s="5">
         <f t="shared" ref="AF8" si="1">(AE8/60)/60</f>
         <v>0.47638888888888886</v>
       </c>
-      <c r="AG8" s="3">
+      <c r="AG8" s="5">
         <f>(((AA8/1000)*AD8)/1000)*AF8</f>
         <v>2.6725416666666666</v>
       </c>
@@ -6253,7 +6246,7 @@
       <c r="D9">
         <v>20359553403</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>20231123173557</v>
       </c>
       <c r="F9" t="b">
@@ -6331,9 +6324,9 @@
       <c r="AD9">
         <v>0</v>
       </c>
-      <c r="AE9" s="4"/>
-      <c r="AF9" s="3"/>
-      <c r="AG9" s="3"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="5"/>
+      <c r="AG9" s="5"/>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
@@ -6348,7 +6341,7 @@
       <c r="D10">
         <v>20374887203</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>20231127023736</v>
       </c>
       <c r="F10" t="b">
@@ -6426,15 +6419,15 @@
       <c r="AD10" s="1">
         <v>204</v>
       </c>
-      <c r="AE10" s="3">
+      <c r="AE10" s="5">
         <f>AB11-AB10</f>
         <v>39560</v>
       </c>
-      <c r="AF10" s="3">
+      <c r="AF10" s="5">
         <f t="shared" ref="AF10" si="2">(AE10/60)/60</f>
         <v>10.988888888888889</v>
       </c>
-      <c r="AG10" s="3">
+      <c r="AG10" s="5">
         <f t="shared" ref="AG10" si="3">(((AA10/1000)*AD10)/1000)*AF10</f>
         <v>61.647666666666673</v>
       </c>
@@ -6452,7 +6445,7 @@
       <c r="D11">
         <v>20374887203</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <v>20231127023736</v>
       </c>
       <c r="F11" t="b">
@@ -6530,9 +6523,9 @@
       <c r="AD11">
         <v>0</v>
       </c>
-      <c r="AE11" s="3"/>
-      <c r="AF11" s="3"/>
-      <c r="AG11" s="3"/>
+      <c r="AE11" s="5"/>
+      <c r="AF11" s="5"/>
+      <c r="AG11" s="5"/>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
@@ -6547,7 +6540,7 @@
       <c r="D12">
         <v>20397123102</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="3">
         <v>20231130120125</v>
       </c>
       <c r="F12" t="b">
@@ -6625,15 +6618,15 @@
       <c r="AD12" s="1">
         <v>204</v>
       </c>
-      <c r="AE12" s="3">
+      <c r="AE12" s="5">
         <f>AB13-AB12</f>
         <v>946</v>
       </c>
-      <c r="AF12" s="3">
+      <c r="AF12" s="5">
         <f t="shared" ref="AF12" si="4">(AE12/60)/60</f>
         <v>0.26277777777777778</v>
       </c>
-      <c r="AG12" s="3">
+      <c r="AG12" s="5">
         <f t="shared" ref="AG12" si="5">(((AA12/1000)*AD12)/1000)*AF12</f>
         <v>1.4741833333333334</v>
       </c>
@@ -6651,7 +6644,7 @@
       <c r="D13">
         <v>20397123102</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="3">
         <v>20231130120125</v>
       </c>
       <c r="F13" t="b">
@@ -6729,9 +6722,9 @@
       <c r="AD13" s="1">
         <v>0</v>
       </c>
-      <c r="AE13" s="3"/>
-      <c r="AF13" s="3"/>
-      <c r="AG13" s="3"/>
+      <c r="AE13" s="5"/>
+      <c r="AF13" s="5"/>
+      <c r="AG13" s="5"/>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
@@ -6746,7 +6739,7 @@
       <c r="D14">
         <v>20426785003</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="3">
         <v>20231203172822</v>
       </c>
       <c r="F14" t="b">
@@ -6824,15 +6817,15 @@
       <c r="AD14" s="1">
         <v>204</v>
       </c>
-      <c r="AE14" s="4">
+      <c r="AE14" s="6">
         <f>AB15-AB14</f>
         <v>27807</v>
       </c>
-      <c r="AF14" s="3">
+      <c r="AF14" s="5">
         <f t="shared" ref="AF14" si="6">(AE14/60)/60</f>
         <v>7.7241666666666662</v>
       </c>
-      <c r="AG14" s="3">
+      <c r="AG14" s="5">
         <f t="shared" ref="AG14" si="7">(((AA14/1000)*AD14)/1000)*AF14</f>
         <v>43.332574999999999</v>
       </c>
@@ -6850,7 +6843,7 @@
       <c r="D15">
         <v>20426785003</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="3">
         <v>20231203172822</v>
       </c>
       <c r="F15" t="b">
@@ -6928,9 +6921,9 @@
       <c r="AD15">
         <v>0</v>
       </c>
-      <c r="AE15" s="4"/>
-      <c r="AF15" s="3"/>
-      <c r="AG15" s="3"/>
+      <c r="AE15" s="6"/>
+      <c r="AF15" s="5"/>
+      <c r="AG15" s="5"/>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
@@ -6945,7 +6938,7 @@
       <c r="D16">
         <v>20427933703</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="3">
         <v>20231204021353</v>
       </c>
       <c r="F16" t="b">
@@ -7023,15 +7016,15 @@
       <c r="AD16" s="1">
         <v>204</v>
       </c>
-      <c r="AE16" s="3">
+      <c r="AE16" s="5">
         <f>AB17-AB16</f>
         <v>38136</v>
       </c>
-      <c r="AF16" s="3">
+      <c r="AF16" s="5">
         <f t="shared" ref="AF16" si="8">(AE16/60)/60</f>
         <v>10.593333333333334</v>
       </c>
-      <c r="AG16" s="3">
+      <c r="AG16" s="5">
         <f t="shared" ref="AG16" si="9">(((AA16/1000)*AD16)/1000)*AF16</f>
         <v>59.428600000000003</v>
       </c>
@@ -7049,7 +7042,7 @@
       <c r="D17">
         <v>20427933703</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="3">
         <v>20231204021353</v>
       </c>
       <c r="F17" t="b">
@@ -7127,9 +7120,9 @@
       <c r="AD17">
         <v>0</v>
       </c>
-      <c r="AE17" s="3"/>
-      <c r="AF17" s="3"/>
-      <c r="AG17" s="3"/>
+      <c r="AE17" s="5"/>
+      <c r="AF17" s="5"/>
+      <c r="AG17" s="5"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
@@ -7144,7 +7137,7 @@
       <c r="D18">
         <v>20476569402</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="3">
         <v>20231210183640</v>
       </c>
       <c r="F18" t="b">
@@ -7222,15 +7215,15 @@
       <c r="AD18" s="1">
         <v>204</v>
       </c>
-      <c r="AE18" s="4">
+      <c r="AE18" s="6">
         <f>AB19-AB18</f>
         <v>61135</v>
       </c>
-      <c r="AF18" s="3">
+      <c r="AF18" s="5">
         <f t="shared" ref="AF18" si="10">(AE18/60)/60</f>
         <v>16.981944444444444</v>
       </c>
-      <c r="AG18" s="3">
+      <c r="AG18" s="5">
         <f t="shared" ref="AG18" si="11">(((AA18/1000)*AD18)/1000)*AF18</f>
         <v>95.268708333333336</v>
       </c>
@@ -7248,7 +7241,7 @@
       <c r="D19">
         <v>20476569402</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="3">
         <v>20231210183640</v>
       </c>
       <c r="F19" t="b">
@@ -7326,9 +7319,9 @@
       <c r="AD19">
         <v>0</v>
       </c>
-      <c r="AE19" s="4"/>
-      <c r="AF19" s="3"/>
-      <c r="AG19" s="3"/>
+      <c r="AE19" s="6"/>
+      <c r="AF19" s="5"/>
+      <c r="AG19" s="5"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
@@ -7343,7 +7336,7 @@
       <c r="D20">
         <v>20484061503</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="3">
         <v>20231212013149</v>
       </c>
       <c r="F20" t="b">
@@ -7421,15 +7414,15 @@
       <c r="AD20" s="1">
         <v>204</v>
       </c>
-      <c r="AE20" s="3">
+      <c r="AE20" s="5">
         <f>AB21-AB20</f>
         <v>33934</v>
       </c>
-      <c r="AF20" s="3">
+      <c r="AF20" s="5">
         <f t="shared" ref="AF20" si="12">(AE20/60)/60</f>
         <v>9.426111111111112</v>
       </c>
-      <c r="AG20" s="3">
+      <c r="AG20" s="5">
         <f t="shared" ref="AG20" si="13">(((AA20/1000)*AD20)/1000)*AF20</f>
         <v>52.880483333333345</v>
       </c>
@@ -7447,7 +7440,7 @@
       <c r="D21">
         <v>20484061503</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="3">
         <v>20231212013149</v>
       </c>
       <c r="F21" t="b">
@@ -7525,33 +7518,18 @@
       <c r="AD21">
         <v>0</v>
       </c>
-      <c r="AE21" s="3"/>
-      <c r="AF21" s="3"/>
-      <c r="AG21" s="3"/>
+      <c r="AE21" s="5"/>
+      <c r="AF21" s="5"/>
+      <c r="AG21" s="5"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="AE22" s="6"/>
+      <c r="AE22" s="4"/>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="AE23" s="6"/>
+      <c r="AE23" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="AG12:AG13"/>
-    <mergeCell ref="AG14:AG15"/>
-    <mergeCell ref="AG16:AG17"/>
-    <mergeCell ref="AG18:AG19"/>
-    <mergeCell ref="AG20:AG21"/>
-    <mergeCell ref="AF12:AF13"/>
-    <mergeCell ref="AF14:AF15"/>
-    <mergeCell ref="AF16:AF17"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AF20:AF21"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AG4:AG5"/>
-    <mergeCell ref="AG6:AG7"/>
-    <mergeCell ref="AG8:AG9"/>
-    <mergeCell ref="AG10:AG11"/>
     <mergeCell ref="AE14:AE15"/>
     <mergeCell ref="AE16:AE17"/>
     <mergeCell ref="AE18:AE19"/>
@@ -7567,6 +7545,21 @@
     <mergeCell ref="AE8:AE9"/>
     <mergeCell ref="AE10:AE11"/>
     <mergeCell ref="AE12:AE13"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AG4:AG5"/>
+    <mergeCell ref="AG6:AG7"/>
+    <mergeCell ref="AG8:AG9"/>
+    <mergeCell ref="AG10:AG11"/>
+    <mergeCell ref="AF12:AF13"/>
+    <mergeCell ref="AF14:AF15"/>
+    <mergeCell ref="AF16:AF17"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AF20:AF21"/>
+    <mergeCell ref="AG12:AG13"/>
+    <mergeCell ref="AG14:AG15"/>
+    <mergeCell ref="AG16:AG17"/>
+    <mergeCell ref="AG18:AG19"/>
+    <mergeCell ref="AG20:AG21"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H21">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="ff^03">

</xml_diff>